<commit_message>
Add branch analysis based on skan
</commit_message>
<xml_diff>
--- a/test/trait.xlsx
+++ b/test/trait.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,1737 @@
         <v>0.03033984992984335</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D3" t="n">
+        <v>343</v>
+      </c>
+      <c r="E3" t="n">
+        <v>282</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D4" t="n">
+        <v>343</v>
+      </c>
+      <c r="E4" t="n">
+        <v>282</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D5" t="n">
+        <v>343</v>
+      </c>
+      <c r="E5" t="n">
+        <v>282</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D6" t="n">
+        <v>343</v>
+      </c>
+      <c r="E6" t="n">
+        <v>282</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D7" t="n">
+        <v>343</v>
+      </c>
+      <c r="E7" t="n">
+        <v>282</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D8" t="n">
+        <v>343</v>
+      </c>
+      <c r="E8" t="n">
+        <v>282</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D9" t="n">
+        <v>343</v>
+      </c>
+      <c r="E9" t="n">
+        <v>282</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D10" t="n">
+        <v>343</v>
+      </c>
+      <c r="E10" t="n">
+        <v>282</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D11" t="n">
+        <v>343</v>
+      </c>
+      <c r="E11" t="n">
+        <v>282</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D12" t="n">
+        <v>343</v>
+      </c>
+      <c r="E12" t="n">
+        <v>282</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D13" t="n">
+        <v>343</v>
+      </c>
+      <c r="E13" t="n">
+        <v>282</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D14" t="n">
+        <v>343</v>
+      </c>
+      <c r="E14" t="n">
+        <v>282</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D15" t="n">
+        <v>343</v>
+      </c>
+      <c r="E15" t="n">
+        <v>282</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D16" t="n">
+        <v>343</v>
+      </c>
+      <c r="E16" t="n">
+        <v>282</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D17" t="n">
+        <v>343</v>
+      </c>
+      <c r="E17" t="n">
+        <v>282</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D18" t="n">
+        <v>343</v>
+      </c>
+      <c r="E18" t="n">
+        <v>282</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D19" t="n">
+        <v>343</v>
+      </c>
+      <c r="E19" t="n">
+        <v>282</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D20" t="n">
+        <v>343</v>
+      </c>
+      <c r="E20" t="n">
+        <v>282</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.01120717025436148</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D21" t="n">
+        <v>343</v>
+      </c>
+      <c r="E21" t="n">
+        <v>282</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.09415256353173122</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D22" t="n">
+        <v>343</v>
+      </c>
+      <c r="E22" t="n">
+        <v>282</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.01120717025436148</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D23" t="n">
+        <v>343</v>
+      </c>
+      <c r="E23" t="n">
+        <v>282</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.09415256353173122</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D24" t="n">
+        <v>343</v>
+      </c>
+      <c r="E24" t="n">
+        <v>282</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.09415256353173122</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D25" t="n">
+        <v>343</v>
+      </c>
+      <c r="E25" t="n">
+        <v>282</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.09415256353173122</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D26" t="n">
+        <v>343</v>
+      </c>
+      <c r="E26" t="n">
+        <v>282</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.058241835046448</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D27" t="n">
+        <v>343</v>
+      </c>
+      <c r="E27" t="n">
+        <v>282</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D28" t="n">
+        <v>343</v>
+      </c>
+      <c r="E28" t="n">
+        <v>282</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D29" t="n">
+        <v>343</v>
+      </c>
+      <c r="E29" t="n">
+        <v>282</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D30" t="n">
+        <v>343</v>
+      </c>
+      <c r="E30" t="n">
+        <v>282</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D31" t="n">
+        <v>343</v>
+      </c>
+      <c r="E31" t="n">
+        <v>282</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D32" t="n">
+        <v>343</v>
+      </c>
+      <c r="E32" t="n">
+        <v>282</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D33" t="n">
+        <v>343</v>
+      </c>
+      <c r="E33" t="n">
+        <v>282</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D34" t="n">
+        <v>343</v>
+      </c>
+      <c r="E34" t="n">
+        <v>282</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D35" t="n">
+        <v>343</v>
+      </c>
+      <c r="E35" t="n">
+        <v>282</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D36" t="n">
+        <v>343</v>
+      </c>
+      <c r="E36" t="n">
+        <v>282</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D37" t="n">
+        <v>343</v>
+      </c>
+      <c r="E37" t="n">
+        <v>282</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D38" t="n">
+        <v>343</v>
+      </c>
+      <c r="E38" t="n">
+        <v>282</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D39" t="n">
+        <v>343</v>
+      </c>
+      <c r="E39" t="n">
+        <v>282</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D40" t="n">
+        <v>343</v>
+      </c>
+      <c r="E40" t="n">
+        <v>282</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D41" t="n">
+        <v>343</v>
+      </c>
+      <c r="E41" t="n">
+        <v>282</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D42" t="n">
+        <v>343</v>
+      </c>
+      <c r="E42" t="n">
+        <v>282</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D43" t="n">
+        <v>343</v>
+      </c>
+      <c r="E43" t="n">
+        <v>282</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D44" t="n">
+        <v>343</v>
+      </c>
+      <c r="E44" t="n">
+        <v>282</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D45" t="n">
+        <v>343</v>
+      </c>
+      <c r="E45" t="n">
+        <v>282</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D46" t="n">
+        <v>343</v>
+      </c>
+      <c r="E46" t="n">
+        <v>282</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D47" t="n">
+        <v>343</v>
+      </c>
+      <c r="E47" t="n">
+        <v>282</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D48" t="n">
+        <v>343</v>
+      </c>
+      <c r="E48" t="n">
+        <v>282</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D49" t="n">
+        <v>343</v>
+      </c>
+      <c r="E49" t="n">
+        <v>282</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D50" t="n">
+        <v>343</v>
+      </c>
+      <c r="E50" t="n">
+        <v>282</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D51" t="n">
+        <v>343</v>
+      </c>
+      <c r="E51" t="n">
+        <v>282</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D52" t="n">
+        <v>343</v>
+      </c>
+      <c r="E52" t="n">
+        <v>282</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D53" t="n">
+        <v>343</v>
+      </c>
+      <c r="E53" t="n">
+        <v>282</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>01.jpg</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>36482</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.4596997246741137</v>
+      </c>
+      <c r="D54" t="n">
+        <v>378</v>
+      </c>
+      <c r="E54" t="n">
+        <v>347</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.04736790425627412</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>02.jpg</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>85107</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.5657431165826874</v>
+      </c>
+      <c r="D55" t="n">
+        <v>548</v>
+      </c>
+      <c r="E55" t="n">
+        <v>434</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.04603633387935394</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>03.jpg</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>69052</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.4309124720741859</v>
+      </c>
+      <c r="D56" t="n">
+        <v>452</v>
+      </c>
+      <c r="E56" t="n">
+        <v>533</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.05275747084535395</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>04.jpg</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>44725.5</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.5537253008468281</v>
+      </c>
+      <c r="D57" t="n">
+        <v>412</v>
+      </c>
+      <c r="E57" t="n">
+        <v>394</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.05015314860587732</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D58" t="n">
+        <v>343</v>
+      </c>
+      <c r="E58" t="n">
+        <v>282</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.09945255789024728</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D59" t="n">
+        <v>343</v>
+      </c>
+      <c r="E59" t="n">
+        <v>282</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D60" t="n">
+        <v>343</v>
+      </c>
+      <c r="E60" t="n">
+        <v>282</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D61" t="n">
+        <v>343</v>
+      </c>
+      <c r="E61" t="n">
+        <v>282</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.0316011453310757</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D62" t="n">
+        <v>343</v>
+      </c>
+      <c r="E62" t="n">
+        <v>282</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.0316011453310757</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D63" t="n">
+        <v>343</v>
+      </c>
+      <c r="E63" t="n">
+        <v>282</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0316011453310757</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>01.jpg</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>36482</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.4596997246741137</v>
+      </c>
+      <c r="D64" t="n">
+        <v>378</v>
+      </c>
+      <c r="E64" t="n">
+        <v>347</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.01689441067234683</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>02.jpg</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>85107</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.5657431165826874</v>
+      </c>
+      <c r="D65" t="n">
+        <v>548</v>
+      </c>
+      <c r="E65" t="n">
+        <v>434</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.0623714389606333</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>03.jpg</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>69052</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.4309124720741859</v>
+      </c>
+      <c r="D66" t="n">
+        <v>452</v>
+      </c>
+      <c r="E66" t="n">
+        <v>533</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.0411448308832538</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>04.jpg</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>44725.5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.5537253008468281</v>
+      </c>
+      <c r="D67" t="n">
+        <v>412</v>
+      </c>
+      <c r="E67" t="n">
+        <v>394</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.09539222855335611</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D68" t="n">
+        <v>343</v>
+      </c>
+      <c r="E68" t="n">
+        <v>282</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.0316011453310757</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D69" t="n">
+        <v>343</v>
+      </c>
+      <c r="E69" t="n">
+        <v>282</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D70" t="n">
+        <v>343</v>
+      </c>
+      <c r="E70" t="n">
+        <v>282</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>01.jpg</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>36482</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.4596997246741137</v>
+      </c>
+      <c r="D71" t="n">
+        <v>378</v>
+      </c>
+      <c r="E71" t="n">
+        <v>347</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.02431618966192055</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>02.jpg</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>85107</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.5657431165826874</v>
+      </c>
+      <c r="D72" t="n">
+        <v>548</v>
+      </c>
+      <c r="E72" t="n">
+        <v>434</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.02228918141274923</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>03.jpg</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>69052</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.4309124720741859</v>
+      </c>
+      <c r="D73" t="n">
+        <v>452</v>
+      </c>
+      <c r="E73" t="n">
+        <v>533</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.02637357401543597</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>04.jpg</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>44725.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.5537253008468281</v>
+      </c>
+      <c r="D74" t="n">
+        <v>412</v>
+      </c>
+      <c r="E74" t="n">
+        <v>394</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.01976068415765238</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D75" t="n">
+        <v>343</v>
+      </c>
+      <c r="E75" t="n">
+        <v>282</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>01.jpg</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>36482</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.4596997246741137</v>
+      </c>
+      <c r="D76" t="n">
+        <v>378</v>
+      </c>
+      <c r="E76" t="n">
+        <v>347</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.02431618966192055</v>
+      </c>
+      <c r="G76" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>02.jpg</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>85107</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.5657431165826874</v>
+      </c>
+      <c r="D77" t="n">
+        <v>548</v>
+      </c>
+      <c r="E77" t="n">
+        <v>434</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.02228918141274923</v>
+      </c>
+      <c r="G77" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>03.jpg</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>69052</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.4309124720741859</v>
+      </c>
+      <c r="D78" t="n">
+        <v>452</v>
+      </c>
+      <c r="E78" t="n">
+        <v>533</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.02637357401543597</v>
+      </c>
+      <c r="G78" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>04.jpg</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>44725.5</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.5537253008468281</v>
+      </c>
+      <c r="D79" t="n">
+        <v>412</v>
+      </c>
+      <c r="E79" t="n">
+        <v>394</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.01976068415765238</v>
+      </c>
+      <c r="G79" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>23384.5</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.4000872563025569</v>
+      </c>
+      <c r="D80" t="n">
+        <v>343</v>
+      </c>
+      <c r="E80" t="n">
+        <v>282</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.03033984992984335</v>
+      </c>
+      <c r="G80" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add marker based ROI detection
</commit_message>
<xml_diff>
--- a/test/trait.xlsx
+++ b/test/trait.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,51 +461,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16C-tray1-2018-07-11.JPG</t>
+          <t>2021-03-08--15-36-20_NewImage_P1.png</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>76641.5</v>
+        <v>3842.5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5117843656408698</v>
+        <v>0.6360701870551233</v>
       </c>
       <c r="D2" t="n">
-        <v>69</v>
+        <v>200</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03998420992191234</v>
+        <v>0.07320878400128331</v>
       </c>
       <c r="G2" t="n">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>16C-tray1-2018-07-11.JPG_label.JPG</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>198839.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.7941715077673955</v>
-      </c>
-      <c r="D3" t="n">
-        <v>369</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.05473938208988647</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1314</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update pipeline seeting for David's data
</commit_message>
<xml_diff>
--- a/test/trait.xlsx
+++ b/test/trait.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +435,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>temp_index</t>
+          <t>solidity</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -455,132 +456,1183 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>number_leaf</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 1</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 2</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 3</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 4</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>color cluster 1 hex value</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>color cluster 2 hex value</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>color cluster 3 hex value</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>color cluster 4 hex value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01.JPG</t>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20344.5</v>
+        <v>31298</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6945648834112867</v>
+        <v>0.6784959406874275</v>
       </c>
       <c r="D2" t="n">
-        <v>211</v>
+        <v>255</v>
       </c>
       <c r="E2" t="n">
-        <v>175</v>
+        <v>276</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03443300232677861</v>
+        <v>0.0333551030243503</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>#b4d78c</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>#a2c27d</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>#91aa71</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>#778962</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>02.JPG</t>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20918</v>
+        <v>32592.5</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7551760862109425</v>
+        <v>0.6873879573974481</v>
       </c>
       <c r="D3" t="n">
-        <v>201</v>
+        <v>256</v>
       </c>
       <c r="E3" t="n">
-        <v>199</v>
+        <v>280</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03003955145646157</v>
+        <v>0.03278798868091025</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>#8fa770</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>#b4d68c</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>#a1bf7d</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>#71825e</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>leaf_index</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>area</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>curvature</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>solidity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>major_axis</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>minor_axis</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 1</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 2</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 3</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>color distribution cluster 4</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>color cluster 1 hex value</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>color cluster 2 hex value</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>color cluster 3 hex value</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>color cluster 4 hex value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>678.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.06606186357860248</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8043864848844102</v>
+      </c>
+      <c r="F2" t="n">
+        <v>16.3015022277832</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14.9105110168457</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>#b1d289</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>#a2bf7d</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>#778961</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>#91a970</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>992.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.04741961760642198</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6354033290653009</v>
+      </c>
+      <c r="F3" t="n">
+        <v>32.23500823974609</v>
+      </c>
+      <c r="G3" t="n">
+        <v>13.62162685394287</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.33</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>#9cbb78</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>#b7dd8e</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>#abcd84</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>#889e70</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03.JPG</t>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17061.5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.698941029475021</v>
+        <v>2024.5</v>
       </c>
       <c r="D4" t="n">
-        <v>189</v>
+        <v>0.03174895852319942</v>
       </c>
       <c r="E4" t="n">
-        <v>190</v>
+        <v>0.6511740109359923</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03488837555740169</v>
+        <v>48.30411911010742</v>
       </c>
       <c r="G4" t="n">
-        <v>6</v>
+        <v>23.65728950500488</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>#c0e395</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>#a6c57f</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>#8da46f</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>#667554</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>04.JPG</t>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15331</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7079985222129861</v>
+        <v>4926.5</v>
       </c>
       <c r="D5" t="n">
-        <v>182</v>
+        <v>0.02397424465805039</v>
       </c>
       <c r="E5" t="n">
-        <v>132</v>
+        <v>0.8857425386551601</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03640216325892939</v>
+        <v>48.83212661743164</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>34.97356414794922</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.48</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>#7e9264</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>#a4c183</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>#91a773</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>#5a6b48</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05.JPG</t>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29040</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6698575630009803</v>
+        <v>5032.5</v>
       </c>
       <c r="D6" t="n">
-        <v>235</v>
+        <v>0.02418413353183936</v>
       </c>
       <c r="E6" t="n">
-        <v>263</v>
+        <v>0.8896844338371784</v>
       </c>
       <c r="F6" t="n">
-        <v>0.03182028044935754</v>
+        <v>46.48287963867188</v>
       </c>
       <c r="G6" t="n">
-        <v>8</v>
+        <v>37.03953552246094</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.43</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>#a6c880</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>#728362</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>#94af75</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>#87a06d</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6110</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.02126447523534697</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8913852213874097</v>
+      </c>
+      <c r="F7" t="n">
+        <v>65.30165100097656</v>
+      </c>
+      <c r="G7" t="n">
+        <v>33.45684432983398</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>#94ac74</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>#9fbb7c</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>#7e9068</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>#acca85</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8128</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.01883242803699147</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8198920663741363</v>
+      </c>
+      <c r="F8" t="n">
+        <v>62.32155990600586</v>
+      </c>
+      <c r="G8" t="n">
+        <v>47.2242317199707</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>#8da66c</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>#9aba76</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>#a7cb7f</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>#778963</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>863</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.06037038690378518</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8290105667627281</v>
+      </c>
+      <c r="F9" t="n">
+        <v>18.23693084716797</v>
+      </c>
+      <c r="G9" t="n">
+        <v>16.34025573730469</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>#a0bb7b</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>#8da36f</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>#70815c</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>#b0d089</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1158.5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.04608350104684451</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6824742268041237</v>
+      </c>
+      <c r="F10" t="n">
+        <v>32.24896621704102</v>
+      </c>
+      <c r="G10" t="n">
+        <v>14.55146217346191</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>#b4d88e</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>#a6c682</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>#6d7b5c</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>#93ad75</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1958.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.03598942669645301</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.7683405256963515</v>
+      </c>
+      <c r="F11" t="n">
+        <v>36.00204086303711</v>
+      </c>
+      <c r="G11" t="n">
+        <v>24.20377731323242</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>#8da470</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>#c2e495</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>#6a7959</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>#a8c67f</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5131.5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.02431957526491579</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.9083104699530932</v>
+      </c>
+      <c r="F12" t="n">
+        <v>45.8285026550293</v>
+      </c>
+      <c r="G12" t="n">
+        <v>37.36833953857422</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>#9db97e</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>#798b62</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>#8ca272</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>#596847</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5582.5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.02293312259366708</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8792723263506064</v>
+      </c>
+      <c r="F13" t="n">
+        <v>51.29258728027344</v>
+      </c>
+      <c r="G13" t="n">
+        <v>37.13410186767578</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>#a0bb7e</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>#798965</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>#aecb88</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>#93aa74</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6269.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.02092283761581119</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8989174851243816</v>
+      </c>
+      <c r="F14" t="n">
+        <v>63.61085891723633</v>
+      </c>
+      <c r="G14" t="n">
+        <v>34.68422698974609</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>#7f9469</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>#8da972</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>#9fbf7f</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>#68765a</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8438</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.018897070644895</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.8250708907793096</v>
+      </c>
+      <c r="F15" t="n">
+        <v>61.43574142456055</v>
+      </c>
+      <c r="G15" t="n">
+        <v>50.07595443725586</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>#8ba36c</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>#a4c880</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>#748561</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>#98b675</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add bbox coordinates output for validation purpose
</commit_message>
<xml_diff>
--- a/test/trait.xlsx
+++ b/test/trait.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,130 +502,65 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31298</v>
+        <v>13354</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6784959406874275</v>
+        <v>0.58416447944007</v>
       </c>
       <c r="D2" t="n">
-        <v>255</v>
+        <v>193</v>
       </c>
       <c r="E2" t="n">
-        <v>276</v>
+        <v>146</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0333551030243503</v>
+        <v>0.05170552984675276</v>
       </c>
       <c r="G2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>#b4d78c</t>
+          <t>#527521</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>#a2c27d</t>
+          <t>#689a2c</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>#91aa71</t>
+          <t>#629a0f</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>#778962</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>32592.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.6873879573974481</v>
-      </c>
-      <c r="D3" t="n">
-        <v>256</v>
-      </c>
-      <c r="E3" t="n">
-        <v>280</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.03278798868091025</v>
-      </c>
-      <c r="G3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>#8fa770</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>#b4d68c</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>#a1bf7d</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>#71825e</t>
+          <t>#375214</t>
         </is>
       </c>
     </row>
@@ -640,7 +575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -728,225 +663,225 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>678.5</v>
+        <v>401</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06606186357860248</v>
+        <v>0.08137249651041048</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8043864848844102</v>
+        <v>0.8468848996832101</v>
       </c>
       <c r="F2" t="n">
-        <v>16.3015022277832</v>
+        <v>14.91173458099365</v>
       </c>
       <c r="G2" t="n">
-        <v>14.9105110168457</v>
+        <v>9.739253044128418</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.31</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.22</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>#b1d289</t>
+          <t>#6ba31f</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>#a2bf7d</t>
+          <t>#629c07</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>#778961</t>
+          <t>#538014</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>#91a970</t>
+          <t>#3b5612</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>992.5</v>
+        <v>524</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04741961760642198</v>
+        <v>0.07537015957185492</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6354033290653009</v>
+        <v>0.9527272727272728</v>
       </c>
       <c r="F3" t="n">
-        <v>32.23500823974609</v>
+        <v>14.51329135894775</v>
       </c>
       <c r="G3" t="n">
-        <v>13.62162685394287</v>
+        <v>12.03914260864258</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.33</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.44</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.33</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0.13</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>#9cbb78</t>
+          <t>#5f9322</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>#b7dd8e</t>
+          <t>#689b32</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>#abcd84</t>
+          <t>#3a541d</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>#889e70</t>
+          <t>#53742e</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>2024.5</v>
+        <v>679.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03174895852319942</v>
+        <v>0.06385325160722903</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6511740109359923</v>
+        <v>0.9017916390179164</v>
       </c>
       <c r="F4" t="n">
-        <v>48.30411911010742</v>
+        <v>18.28932952880859</v>
       </c>
       <c r="G4" t="n">
-        <v>23.65728950500488</v>
+        <v>13.06778526306152</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.52</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.23</t>
+          <t>0.32</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>#c0e395</t>
+          <t>#749e36</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>#a6c57f</t>
+          <t>#364f17</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>#8da46f</t>
+          <t>#668f2f</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>#667554</t>
+          <t>#517026</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>4926.5</v>
+        <v>984.5</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02397424465805039</v>
+        <v>0.05363728343934814</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8857425386551601</v>
+        <v>0.8040016333197223</v>
       </c>
       <c r="F5" t="n">
-        <v>48.83212661743164</v>
+        <v>23.42160415649414</v>
       </c>
       <c r="G5" t="n">
-        <v>34.97356414794922</v>
+        <v>15.24034214019775</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.27</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -956,682 +891,357 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>#7e9264</t>
+          <t>#689737</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>#a4c183</t>
+          <t>#385115</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>#91a773</t>
+          <t>#51711f</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>#5a6b48</t>
+          <t>#5d971d</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5032.5</v>
+        <v>1404.5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02418413353183936</v>
+        <v>0.04624205780978436</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8896844338371784</v>
+        <v>0.9353979353979354</v>
       </c>
       <c r="F6" t="n">
-        <v>46.48287963867188</v>
+        <v>24.68202781677246</v>
       </c>
       <c r="G6" t="n">
-        <v>37.03953552246094</v>
+        <v>18.58641242980957</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.10</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.27</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>#a6c880</t>
+          <t>#314b0d</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>#728362</t>
+          <t>#476919</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>#94af75</t>
+          <t>#5f9424</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>#87a06d</t>
+          <t>#6e9f3b</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>6110</v>
+        <v>1874</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02126447523534697</v>
+        <v>0.04001269099130673</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8913852213874097</v>
+        <v>0.8852149267831837</v>
       </c>
       <c r="F7" t="n">
-        <v>65.30165100097656</v>
+        <v>27.65208625793457</v>
       </c>
       <c r="G7" t="n">
-        <v>33.45684432983398</v>
+        <v>22.92923927307129</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>0.31</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0.38</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.26</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>#94ac74</t>
+          <t>#4f731f</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>#9fbb7c</t>
+          <t>#619813</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>#7e9068</t>
+          <t>#365012</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>#acca85</t>
+          <t>#679b2a</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021-03-12--07-37-00_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>8128</v>
+        <v>2233</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01883242803699147</v>
+        <v>0.03513051977141209</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8198920663741363</v>
+        <v>0.8453530191179254</v>
       </c>
       <c r="F8" t="n">
-        <v>62.32155990600586</v>
+        <v>35.98834991455078</v>
       </c>
       <c r="G8" t="n">
-        <v>47.2242317199707</v>
+        <v>23.91048622131348</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.33</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>#8da66c</t>
+          <t>#314a14</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>#9aba76</t>
+          <t>#5b8026</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>#a7cb7f</t>
+          <t>#67902f</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>#778963</t>
+          <t>#496523</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>863</v>
+        <v>2296.5</v>
       </c>
       <c r="D9" t="n">
-        <v>0.06037038690378518</v>
+        <v>0.0346387995809897</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8290105667627281</v>
+        <v>0.8471043895241608</v>
       </c>
       <c r="F9" t="n">
-        <v>18.23693084716797</v>
+        <v>35.90595245361328</v>
       </c>
       <c r="G9" t="n">
-        <v>16.34025573730469</v>
+        <v>24.001708984375</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.32</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.44</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.10</t>
+          <t>0.30</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>#a0bb7b</t>
+          <t>#50741a</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>#8da36f</t>
+          <t>#6a9e22</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>#70815c</t>
+          <t>#5f9609</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>#b0d089</t>
+          <t>#365014</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
+          <t>ara2013_plant01_frame10_rgb.png</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>1158.5</v>
+        <v>2330.5</v>
       </c>
       <c r="D10" t="n">
-        <v>0.04608350104684451</v>
+        <v>0.03509250933843939</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6824742268041237</v>
+        <v>0.8723563541081789</v>
       </c>
       <c r="F10" t="n">
-        <v>32.24896621704102</v>
+        <v>34.14801788330078</v>
       </c>
       <c r="G10" t="n">
-        <v>14.55146217346191</v>
+        <v>24.66762733459473</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.40</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.38</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>#b4d88e</t>
+          <t>#629f09</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>#a6c682</t>
+          <t>#354e12</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>#6d7b5c</t>
+          <t>#51761c</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>#93ad75</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1958.5</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.03598942669645301</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.7683405256963515</v>
-      </c>
-      <c r="F11" t="n">
-        <v>36.00204086303711</v>
-      </c>
-      <c r="G11" t="n">
-        <v>24.20377731323242</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0.57</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>0.19</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>#8da470</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>#c2e495</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>#6a7959</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>#a8c67f</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5131.5</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.02431957526491579</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.9083104699530932</v>
-      </c>
-      <c r="F12" t="n">
-        <v>45.8285026550293</v>
-      </c>
-      <c r="G12" t="n">
-        <v>37.36833953857422</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>0.19</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>0.54</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>#9db97e</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>#798b62</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>#8ca272</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>#596847</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" t="n">
-        <v>5582.5</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.02293312259366708</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.8792723263506064</v>
-      </c>
-      <c r="F13" t="n">
-        <v>51.29258728027344</v>
-      </c>
-      <c r="G13" t="n">
-        <v>37.13410186767578</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>0.39</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>0.04</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>#a0bb7e</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>#798965</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>#aecb88</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>#93aa74</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>6269.5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.02092283761581119</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.8989174851243816</v>
-      </c>
-      <c r="F14" t="n">
-        <v>63.61085891723633</v>
-      </c>
-      <c r="G14" t="n">
-        <v>34.68422698974609</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>0.15</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>0.09</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>#7f9469</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>#8da972</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>#9fbf7f</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>#68765a</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2021-03-12--11-37-02_NewImage_P1_cropped.png</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>8438</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.018897070644895</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.8250708907793096</v>
-      </c>
-      <c r="F15" t="n">
-        <v>61.43574142456055</v>
-      </c>
-      <c r="G15" t="n">
-        <v>50.07595443725586</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>0.26</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0.32</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>0.04</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>0.37</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>#8ba36c</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>#a4c880</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>#748561</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>#98b675</t>
+          <t>#6aa023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix 3rd party libray update issue, add demo test, images
</commit_message>
<xml_diff>
--- a/test/trait.xlsx
+++ b/test/trait.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="plant morphological traits" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="leaf specific traits" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,87 +480,407 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>color cluster 1 hex value</t>
+          <t>color cluster 1 RGB value</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>color cluster 2 hex value</t>
+          <t>color cluster 2 RGB value</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>color cluster 3 hex value</t>
+          <t>color cluster 3 RGB value</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>color cluster 4 hex value</t>
+          <t>color cluster 4 RGB value</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>color cluster 1 HEX value</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>color cluster 2 HEX value</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>color cluster 3 HEX value</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>color cluster 4 HEX value</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>average HEX value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_01.png</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13354</v>
+        <v>9125</v>
       </c>
       <c r="C2" t="n">
-        <v>0.58416447944007</v>
+        <v>0.5093923577190387</v>
       </c>
       <c r="D2" t="n">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="E2" t="n">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05170552984675276</v>
+        <v>0.04116326584913347</v>
       </c>
       <c r="G2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(0.3333333333333333, 0.4392156862745098, 0.2235294117647059)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>(0.28627450980392155, 0.37254901960784315, 0.19607843137254902)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>(0.22745098039215686, 0.2823529411764706, 0.16862745098039217)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(0.3803921568627451, 0.47843137254901963, 0.2627450980392157)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>#557039</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>#495f32</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>#3a482b</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>#617a43</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0x4ea476</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>day_05.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>32607</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4261266735930057</v>
+      </c>
+      <c r="D3" t="n">
+        <v>395</v>
+      </c>
+      <c r="E3" t="n">
+        <v>283</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.02280853805820268</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>0.16</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>0.41</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(0.19607843137254902, 0.23921568627450981, 0.13333333333333333)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>(0.2980392156862745, 0.3803921568627451, 0.2)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>(0.25098039215686274, 0.3137254901960784, 0.16862745098039217)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(0.34509803921568627, 0.43137254901960786, 0.23137254901960785)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>#323d22</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>#4c6133</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>#40502b</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>#586e3b</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0x45d72e</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>160497</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5577402237257744</v>
+      </c>
+      <c r="D4" t="n">
+        <v>643</v>
+      </c>
+      <c r="E4" t="n">
+        <v>597</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01496435863840818</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>(0.13725490196078433, 0.14901960784313725, 0.10980392156862745)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>(0.3058823529411765, 0.3803921568627451, 0.2196078431372549)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>(0.2627450980392157, 0.3333333333333333, 0.18823529411764706)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>(0.21176470588235294, 0.25882352941176473, 0.15294117647058825)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>#23261c</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>#4e6138</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>#435530</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>#364227</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>0x3ac7aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>295474.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.4435768137176896</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1025</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1033</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.01224972843682125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>0.13</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>#527521</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>#689a2c</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>#629a0f</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>#375214</t>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>(0.3176470588235294, 0.41568627450980394, 0.22745098039215686)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>(0.2196078431372549, 0.26666666666666666, 0.16470588235294117)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>(0.4, 0.5254901960784314, 0.27450980392156865)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>(0.5019607843137255, 0.6470588235294118, 0.3215686274509804)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>#516a3a</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>#38442a</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>#668646</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>#80a552</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0x5c367f</t>
         </is>
       </c>
     </row>
@@ -575,7 +895,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,243 +961,343 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>color cluster 1 hex value</t>
+          <t>color cluster 1 RGB value</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>color cluster 2 hex value</t>
+          <t>color cluster 2 RGB value</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>color cluster 3 hex value</t>
+          <t>color cluster 3 RGB value</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>color cluster 4 hex value</t>
+          <t>color cluster 4 RGB value</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>color cluster 1 HEX value</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>color cluster 2 HEX value</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>color cluster 3 HEX value</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>color cluster 4 HEX value</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>average HEX value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_01.png</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>401</v>
+        <v>1267.5</v>
       </c>
       <c r="D2" t="n">
-        <v>0.08137249651041048</v>
+        <v>0.04867115933808505</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8468848996832101</v>
+        <v>0.9483726150392817</v>
       </c>
       <c r="F2" t="n">
-        <v>14.91173458099365</v>
+        <v>22.62723159790039</v>
       </c>
       <c r="G2" t="n">
-        <v>9.739253044128418</v>
+        <v>19.44040107727051</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.26</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>#6ba31f</t>
+          <t>(0.3058823529411765, 0.4, 0.2)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>#629c07</t>
+          <t>(0.21176470588235294, 0.2627450980392157, 0.16470588235294117)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>#538014</t>
+          <t>(0.34901960784313724, 0.45098039215686275, 0.22745098039215686)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>#3b5612</t>
+          <t>(0.26666666666666666, 0.3411764705882353, 0.17647058823529413)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>#4e6633</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>#36432a</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>#59733a</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>#44572d</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0x489cf1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_01.png</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>524</v>
+        <v>1498.5</v>
       </c>
       <c r="D3" t="n">
-        <v>0.07537015957185492</v>
+        <v>0.04561482625320157</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9527272727272728</v>
+        <v>0.8973053892215569</v>
       </c>
       <c r="F3" t="n">
-        <v>14.51329135894775</v>
+        <v>23.55860137939453</v>
       </c>
       <c r="G3" t="n">
-        <v>12.03914260864258</v>
+        <v>21.24024391174316</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.33</t>
+          <t>0.41</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.38</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>#5f9322</t>
+          <t>(0.3411764705882353, 0.4392156862745098, 0.23137254901960785)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>#689b32</t>
+          <t>(0.27450980392156865, 0.3411764705882353, 0.18823529411764706)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>#3a541d</t>
+          <t>(0.20784313725490197, 0.25882352941176473, 0.1411764705882353)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>#53742e</t>
+          <t>(0.38823529411764707, 0.49411764705882355, 0.27058823529411763)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>#57703b</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>#465730</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>#354224</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>#637e45</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0x4da1f5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_01.png</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>679.5</v>
+        <v>1633.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06385325160722903</v>
+        <v>0.043109606965906</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9017916390179164</v>
+        <v>0.9535901926444834</v>
       </c>
       <c r="F4" t="n">
-        <v>18.28932952880859</v>
+        <v>32.44014358520508</v>
       </c>
       <c r="G4" t="n">
-        <v>13.06778526306152</v>
+        <v>18.28342056274414</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.32</t>
+          <t>0.13</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.20</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>#749e36</t>
+          <t>(0.32941176470588235, 0.43529411764705883, 0.2235294117647059)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>#364f17</t>
+          <t>(0.28627450980392155, 0.3568627450980392, 0.20392156862745098)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>#668f2f</t>
+          <t>(0.21568627450980393, 0.27058823529411763, 0.1568627450980392)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>#517026</t>
+          <t>(0.3764705882352941, 0.47058823529411764, 0.26666666666666666)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>#546f39</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>#495b34</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>#374528</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>#607844</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>0x4d61f6</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_01.png</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>984.5</v>
+        <v>2270</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05363728343934814</v>
+        <v>0.03598717065602308</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8040016333197223</v>
+        <v>0.833180400073408</v>
       </c>
       <c r="F5" t="n">
-        <v>23.42160415649414</v>
+        <v>37.43220520019531</v>
       </c>
       <c r="G5" t="n">
-        <v>15.24034214019775</v>
+        <v>21.65547370910645</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -886,267 +1306,367 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.37</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.28</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>#689737</t>
+          <t>(0.29411764705882354, 0.37254901960784315, 0.21176470588235294)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>#385115</t>
+          <t>(0.3607843137254902, 0.43529411764705883, 0.25098039215686274)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>#51711f</t>
+          <t>(0.24705882352941178, 0.3137254901960784, 0.18823529411764706)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>#5d971d</t>
+          <t>(0.21568627450980393, 0.26666666666666666, 0.16862745098039217)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>#4b5f36</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>#5c6f40</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>#3f5030</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>#37442b</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0x4798b4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_01.png</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1404.5</v>
+        <v>2390.5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04624205780978436</v>
+        <v>0.03243356603245164</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9353979353979354</v>
+        <v>0.7607000795544948</v>
       </c>
       <c r="F6" t="n">
-        <v>24.68202781677246</v>
+        <v>39.95094299316406</v>
       </c>
       <c r="G6" t="n">
-        <v>18.58641242980957</v>
+        <v>26.37479400634766</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>0.19</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.27</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>0.31</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.10</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>#314b0d</t>
+          <t>(0.30196078431372547, 0.403921568627451, 0.19215686274509805)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>#476919</t>
+          <t>(0.27058823529411763, 0.34901960784313724, 0.1803921568627451)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>#5f9424</t>
+          <t>(0.33725490196078434, 0.44313725490196076, 0.21568627450980393)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>#6e9f3b</t>
+          <t>(0.2235294117647059, 0.27450980392156865, 0.17254901960784313)</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>#4d6731</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>#45592e</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>#567137</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>#39462c</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>0x489df0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_05.png</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1874</v>
+        <v>411</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04001269099130673</v>
+        <v>0.01210778654423666</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8852149267831837</v>
+        <v>0.8138613861386138</v>
       </c>
       <c r="F7" t="n">
-        <v>27.65208625793457</v>
+        <v>32.78879547119141</v>
       </c>
       <c r="G7" t="n">
-        <v>22.92923927307129</v>
+        <v>5.079777240753174</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.31</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.28</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>#4f731f</t>
+          <t>(0.21568627450980393, 0.2627450980392157, 0.1450980392156863)</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>#619813</t>
+          <t>(0.17254901960784313, 0.20392156862745098, 0.12549019607843137)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>#365012</t>
+          <t>(0.25098039215686274, 0.3137254901960784, 0.16862745098039217)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>#679b2a</t>
+          <t>(0.2823529411764706, 0.3568627450980392, 0.19607843137254902)</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>#374325</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>#2c3420</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>#40502b</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>#485b32</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>0x3b08a8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_05.png</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>2233</v>
+        <v>1812</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03513051977141209</v>
+        <v>0.03780105351421505</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8453530191179254</v>
+        <v>0.5868825910931174</v>
       </c>
       <c r="F8" t="n">
-        <v>35.98834991455078</v>
+        <v>38.74134063720703</v>
       </c>
       <c r="G8" t="n">
-        <v>23.91048622131348</v>
+        <v>24.8999080657959</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.13</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.33</t>
+          <t>0.10</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>0.43</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>#314a14</t>
+          <t>(0.25098039215686274, 0.3176470588235294, 0.17647058823529413)</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>#5b8026</t>
+          <t>(0.2, 0.24313725490196078, 0.1411764705882353)</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>#67902f</t>
+          <t>(0.29411764705882354, 0.37254901960784315, 0.19607843137254902)</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>#496523</t>
+          <t>(0.3215686274509804, 0.4117647058823529, 0.21176470588235294)</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>#40512d</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>#333e24</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>#4b5f32</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>#526936</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>0x4455ee</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_05.png</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>2296.5</v>
+        <v>3200.5</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0346387995809897</v>
+        <v>0.0282097663787384</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8471043895241608</v>
+        <v>0.7832843857072932</v>
       </c>
       <c r="F9" t="n">
-        <v>35.90595245361328</v>
+        <v>44.16073989868164</v>
       </c>
       <c r="G9" t="n">
-        <v>24.001708984375</v>
+        <v>28.76640701293945</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>0.38</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1156,92 +1676,2392 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>#50741a</t>
+          <t>(0.2196078431372549, 0.2627450980392157, 0.1411764705882353)</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>#6a9e22</t>
+          <t>(0.17254901960784313, 0.21176470588235294, 0.11764705882352941)</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>#5f9609</t>
+          <t>(0.26666666666666666, 0.3333333333333333, 0.1843137254901961)</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>#365014</t>
+          <t>(0.3215686274509804, 0.396078431372549, 0.22745098039215686)</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>#384324</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>#2c361e</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>#44552f</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>#52653a</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>0x3eccea</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ara2013_plant01_frame10_rgb.png</t>
+          <t>day_05.png</t>
         </is>
       </c>
       <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5760.5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.02168864453372248</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8069622469706521</v>
+      </c>
+      <c r="F10" t="n">
+        <v>58.44460678100586</v>
+      </c>
+      <c r="G10" t="n">
+        <v>37.17020797729492</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>(0.21568627450980393, 0.2627450980392157, 0.14901960784313725)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>(0.2784313725490196, 0.34509803921568627, 0.1843137254901961)</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>(0.3254901960784314, 0.403921568627451, 0.21568627450980393)</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>(0.36470588235294116, 0.45098039215686275, 0.24313725490196078)</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>#374326</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>#47582f</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>#536737</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>#5d733e</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>0x4bdd72</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>day_05.png</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6276.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.02203642073026176</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.8943431176973496</v>
+      </c>
+      <c r="F11" t="n">
+        <v>49.80890274047852</v>
+      </c>
+      <c r="G11" t="n">
+        <v>42.857421875</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>(0.40784313725490196, 0.47843137254901963, 0.2627450980392157)</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>(0.3568627450980392, 0.43137254901960786, 0.23921568627450981)</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>(0.2901960784313726, 0.34509803921568627, 0.20392156862745098)</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>(0.21176470588235294, 0.24705882352941178, 0.17254901960784313)</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>#687a43</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>#5b6e3d</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>#4a5834</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>#363f2c</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>0x511ff8</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>day_05.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7356.5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01998294351415143</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8432485098578634</v>
+      </c>
+      <c r="F12" t="n">
+        <v>61.56542587280273</v>
+      </c>
+      <c r="G12" t="n">
+        <v>41.50372314453125</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>(0.2980392156862745, 0.3803921568627451, 0.2)</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>(0.2549019607843137, 0.3254901960784314, 0.16862745098039217)</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>(0.2235294117647059, 0.2784313725490196, 0.1450980392156863)</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>(0.1843137254901961, 0.22745098039215686, 0.12156862745098039)</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>#4c6133</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>#41532b</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>#394725</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>#2f3a1f</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>0x3d8d68</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>day_05.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7708.5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.01783315119209296</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.7685826810907822</v>
+      </c>
+      <c r="F13" t="n">
+        <v>71.96849060058594</v>
+      </c>
+      <c r="G13" t="n">
+        <v>44.25952911376953</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.48</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>(0.32941176470588235, 0.42745098039215684, 0.2196078431372549)</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>(0.29411764705882354, 0.3843137254901961, 0.19607843137254902)</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>(0.24705882352941178, 0.30980392156862746, 0.16862745098039217)</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>(0.18823529411764706, 0.22745098039215686, 0.1411764705882353)</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>#546d38</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>#4b6232</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>#3f4f2b</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>#303a24</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>0x43d62e</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4156</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.026263675763964</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8603664216954766</v>
+      </c>
+      <c r="F14" t="n">
+        <v>42.58903121948242</v>
+      </c>
+      <c r="G14" t="n">
+        <v>35.10588836669922</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.46</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>(0.13333333333333333, 0.13725490196078433, 0.10980392156862745)</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>(0.3058823529411765, 0.3843137254901961, 0.2235294117647059)</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>(0.27058823529411763, 0.3411764705882353, 0.19607843137254902)</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>(0.2196078431372549, 0.26666666666666666, 0.16470588235294117)</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>#22231c</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>#4e6239</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>#455732</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>#38442a</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>0x3b882c</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10279</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.01741446556873525</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.9193685434461786</v>
+      </c>
+      <c r="F15" t="n">
+        <v>62.71366500854492</v>
+      </c>
+      <c r="G15" t="n">
+        <v>53.01925277709961</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.43</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>(0.28627450980392155, 0.34901960784313724, 0.20784313725490197)</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>(0.23921568627450981, 0.2784313725490196, 0.1803921568627451)</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>(0.3176470588235294, 0.38823529411764707, 0.23137254901960785)</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>(0.14901960784313725, 0.15294117647058825, 0.12549019607843137)</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>#495935</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>#3d472e</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>#51633b</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>#262720</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>0x3f8aaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>11436</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0163778788125024</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.974479144476162</v>
+      </c>
+      <c r="F16" t="n">
+        <v>82.78746795654297</v>
+      </c>
+      <c r="G16" t="n">
+        <v>54.60103225708008</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>(0.17647058823529413, 0.2, 0.1411764705882353)</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>(0.29411764705882354, 0.3803921568627451, 0.21568627450980393)</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>(0.2235294117647059, 0.2784313725490196, 0.16470588235294117)</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>(0.25882352941176473, 0.32941176470588235, 0.19215686274509805)</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>#2d3324</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>#4b6137</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>#39472a</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>#425431</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>0x3d0bed</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="n">
+        <v>12314</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0155105650048595</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.8129662639466561</v>
+      </c>
+      <c r="F17" t="n">
+        <v>81.41043090820312</v>
+      </c>
+      <c r="G17" t="n">
+        <v>56.57536697387695</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>(0.20392156862745098, 0.23529411764705882, 0.1568627450980392)</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>(0.13333333333333333, 0.1411764705882353, 0.10588235294117647)</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>(0.2549019607843137, 0.3137254901960784, 0.19607843137254902)</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>(0.29411764705882354, 0.3568627450980392, 0.22745098039215686)</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>#343c28</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>#22241b</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>#415032</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>#4b5b3a</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>0x38c2eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>15089</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.01441915663461237</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.9473849438061154</v>
+      </c>
+      <c r="F18" t="n">
+        <v>80.90633392333984</v>
+      </c>
+      <c r="G18" t="n">
+        <v>59.5616569519043</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>(0.2823529411764706, 0.34509803921568627, 0.2)</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>(0.12941176470588237, 0.13333333333333333, 0.10196078431372549)</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>(0.24313725490196078, 0.2980392156862745, 0.17254901960784313)</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>(0.2, 0.24313725490196078, 0.1411764705882353)</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>#485833</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>#21221a</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>#3e4c2c</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>#333e24</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>0x36c127</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>18271.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01268856972535159</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.9173130506815272</v>
+      </c>
+      <c r="F19" t="n">
+        <v>93.80417633056641</v>
+      </c>
+      <c r="G19" t="n">
+        <v>63.69834136962891</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>(0.24313725490196078, 0.30196078431372547, 0.1803921568627451)</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>(0.19607843137254902, 0.23529411764705882, 0.14901960784313725)</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>(0.28627450980392155, 0.3607843137254902, 0.21176470588235294)</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>(0.12941176470588237, 0.13333333333333333, 0.10196078431372549)</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>#3e4d2e</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>#323c26</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>#495c36</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>#21221a</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>0x36c1e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>18708.5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.012941259443281</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.9500317379713089</v>
+      </c>
+      <c r="F20" t="n">
+        <v>83.58510589599609</v>
+      </c>
+      <c r="G20" t="n">
+        <v>73.48583221435547</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.48</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>(0.1450980392156863, 0.1450980392156863, 0.12549019607843137)</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>(0.2196078431372549, 0.27450980392156865, 0.1568627450980392)</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>(0.25882352941176473, 0.3333333333333333, 0.1843137254901961)</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>(0.29411764705882354, 0.3764705882352941, 0.20784313725490197)</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>#252520</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>#384628</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>#42552f</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>#4b6035</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>0x3ac82b</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>7</v>
+      </c>
+      <c r="C21" t="n">
+        <v>20090.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0127807127816872</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.9382822716233887</v>
+      </c>
+      <c r="F21" t="n">
+        <v>106.0106735229492</v>
+      </c>
+      <c r="G21" t="n">
+        <v>60.08168411254883</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.33</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>(0.13333333333333333, 0.1450980392156863, 0.10588235294117647)</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>(0.2549019607843137, 0.3215686274509804, 0.1803921568627451)</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>(0.2, 0.24705882352941178, 0.1411764705882353)</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>(0.2980392156862745, 0.3764705882352941, 0.21176470588235294)</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>#22251b</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>#41522e</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>#333f24</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>#4c6036</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>0x38c5a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>8</v>
       </c>
-      <c r="C10" t="n">
-        <v>2330.5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.03509250933843939</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.8723563541081789</v>
-      </c>
-      <c r="F10" t="n">
-        <v>34.14801788330078</v>
-      </c>
-      <c r="G10" t="n">
-        <v>24.66762733459473</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="C22" t="n">
+        <v>22389.5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.01136149266163736</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.8594157838169815</v>
+      </c>
+      <c r="F22" t="n">
+        <v>93.6903076171875</v>
+      </c>
+      <c r="G22" t="n">
+        <v>92.94058990478516</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0.49</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>(0.3058823529411765, 0.396078431372549, 0.21568627450980393)</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>(0.2784313725490196, 0.3568627450980392, 0.19607843137254902)</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>(0.2235294117647059, 0.27058823529411763, 0.16470588235294117)</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>(0.1411764705882353, 0.1411764705882353, 0.12156862745098039)</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>#4e6537</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>#475b32</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>#39452a</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>#24241f</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>0x3cca6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>day_10.png</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>9</v>
+      </c>
+      <c r="C23" t="n">
+        <v>26006</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.009885809987451121</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.862696964670758</v>
+      </c>
+      <c r="F23" t="n">
+        <v>148.6200561523438</v>
+      </c>
+      <c r="G23" t="n">
+        <v>64.08065795898438</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>(0.2823529411764706, 0.34901960784313724, 0.2)</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>(0.14901960784313725, 0.17254901960784313, 0.10980392156862745)</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>(0.22745098039215686, 0.2784313725490196, 0.1568627450980392)</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>(0.4392156862745098, 0.4588235294117647, 0.3333333333333333)</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>#485933</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>#262c1c</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>#3a4728</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>#707555</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>0x465073</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4916</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.02285990903708036</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.8904184024633218</v>
+      </c>
+      <c r="F24" t="n">
+        <v>56.48112869262695</v>
+      </c>
+      <c r="G24" t="n">
+        <v>30.44016265869141</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>0.11</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>(0.2549019607843137, 0.33725490196078434, 0.18823529411764706)</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>(0.18823529411764706, 0.23137254901960785, 0.1450980392156863)</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>(0.34901960784313724, 0.4627450980392157, 0.27058823529411763)</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>(0.3058823529411765, 0.403921568627451, 0.23529411764705882)</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>#415630</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>#303b25</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>#597645</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>#4e673c</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>0x465bb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>5133.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.02257960454787824</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9739138683361791</v>
+      </c>
+      <c r="F25" t="n">
+        <v>48.48344802856445</v>
+      </c>
+      <c r="G25" t="n">
+        <v>37.12453079223633</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>(0.27058823529411763, 0.3568627450980392, 0.1843137254901961)</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>(0.41568627450980394, 0.5490196078431373, 0.2901960784313726)</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>(0.35294117647058826, 0.47058823529411764, 0.23921568627450981)</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>(0.18823529411764706, 0.22745098039215686, 0.1450980392156863)</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>#455b2f</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>#6a8c4a</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>#5a783d</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>#303a25</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>0x4ea676</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>12627</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.01477035991986853</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9633415983215716</v>
+      </c>
+      <c r="F26" t="n">
+        <v>81.31620025634766</v>
+      </c>
+      <c r="G26" t="n">
+        <v>62.2355842590332</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>(0.47843137254901963, 0.6235294117647059, 0.3137254901960784)</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>(0.4117647058823529, 0.5450980392156862, 0.27450980392156865)</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>(0.3411764705882353, 0.4470588235294118, 0.23137254901960785)</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>(0.21176470588235294, 0.25098039215686274, 0.17254901960784313)</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>#7a9f50</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>#698b46</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>#57723b</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>#36402c</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>0x5c773f</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" t="n">
+        <v>14875</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01372577059036936</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.8390918065153011</v>
+      </c>
+      <c r="F27" t="n">
+        <v>145.2072906494141</v>
+      </c>
+      <c r="G27" t="n">
+        <v>63.96603012084961</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>(0.23529411764705882, 0.27450980392156865, 0.1803921568627451)</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>(0.44313725490196076, 0.5725490196078431, 0.27450980392156865)</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>(0.5607843137254902, 0.7058823529411765, 0.33725490196078434)</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>(0.34901960784313724, 0.43529411764705883, 0.23921568627450981)</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>#3c462e</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>#719246</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>#8fb456</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>#596f3d</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>0x65bf01</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" t="n">
+        <v>18404.5</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01225761891892937</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.9544664851549333</v>
+      </c>
+      <c r="F28" t="n">
+        <v>98.65715026855469</v>
+      </c>
+      <c r="G28" t="n">
+        <v>67.04881286621094</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>0.15</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>(0.5294117647058824, 0.6784313725490196, 0.32941176470588235)</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>(0.34509803921568627, 0.43529411764705883, 0.23529411764705882)</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>(0.4392156862745098, 0.5568627450980392, 0.2901960784313726)</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>(0.21568627450980393, 0.24313725490196078, 0.1803921568627451)</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>#87ad54</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>#586f3c</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>#708e4a</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>#373e2e</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>0x61fa42</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>19398</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0122221444605071</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.9108538961801235</v>
+      </c>
+      <c r="F29" t="n">
+        <v>95.51164245605469</v>
+      </c>
+      <c r="G29" t="n">
+        <v>70.33993530273438</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>(0.403921568627451, 0.5372549019607843, 0.3058823529411765)</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>(0.28627450980392155, 0.3764705882352941, 0.2)</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>(0.3568627450980392, 0.47058823529411764, 0.25882352941176473)</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>(0.1607843137254902, 0.17254901960784313, 0.13333333333333333)</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>#67894e</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>#496033</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>#5b7842</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>#292c22</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>0x4d6379</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>6</v>
+      </c>
+      <c r="C30" t="n">
+        <v>24242</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.005523891296027148</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.801560665928216</v>
+      </c>
+      <c r="F30" t="n">
+        <v>482.2804870605469</v>
+      </c>
+      <c r="G30" t="n">
+        <v>72.26915740966797</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>0.39</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>#629f09</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>#354e12</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>#51761c</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>#6aa023</t>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>(0.3333333333333333, 0.45098039215686275, 0.23529411764705882)</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>(0.27058823529411763, 0.3607843137254902, 0.1843137254901961)</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>(0.1568627450980392, 0.16470588235294117, 0.12941176470588237)</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>(0.39215686274509803, 0.5294117647058824, 0.28627450980392155)</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>#55733c</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>#455c2f</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>#282a21</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>#648749</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>0x49e035</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>7</v>
+      </c>
+      <c r="C31" t="n">
+        <v>24688.5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01112855615399692</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.9690505161518232</v>
+      </c>
+      <c r="F31" t="n">
+        <v>186.6820220947266</v>
+      </c>
+      <c r="G31" t="n">
+        <v>60.60490036010742</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>(0.35294117647058826, 0.4470588235294118, 0.23529411764705882)</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>(0.45098039215686275, 0.5764705882352941, 0.2823529411764706)</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>(0.23529411764705882, 0.2823529411764706, 0.1803921568627451)</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>(0.5411764705882353, 0.6862745098039216, 0.32941176470588235)</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>#5a723c</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>#739348</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>#3c482e</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>#8aaf54</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>0x653f41</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>8</v>
+      </c>
+      <c r="C32" t="n">
+        <v>35969</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.009130508232360618</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.8573335399063271</v>
+      </c>
+      <c r="F32" t="n">
+        <v>153.0662689208984</v>
+      </c>
+      <c r="G32" t="n">
+        <v>79.45516204833984</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>0.49</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>0.44</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>(0.4745098039215686, 0.5843137254901961, 0.2980392156862745)</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>(0.13725490196078433, 0.14901960784313725, 0.11372549019607843)</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>(0.2784313725490196, 0.35294117647058826, 0.21568627450980393)</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>(0.2196078431372549, 0.2784313725490196, 0.1607843137254902)</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>#79954c</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>#23261d</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>#475a37</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>#384729</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>0x471732</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>40986</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.007843198796268739</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.9002767649255371</v>
+      </c>
+      <c r="F33" t="n">
+        <v>190.6384735107422</v>
+      </c>
+      <c r="G33" t="n">
+        <v>73.11412048339844</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>(0.3254901960784314, 0.43137254901960786, 0.24313725490196078)</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>(0.27450980392156865, 0.35294117647058826, 0.2)</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>(0.36470588235294116, 0.48627450980392156, 0.27450980392156865)</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>(0.15294117647058825, 0.17254901960784313, 0.12941176470588237)</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>#536e3e</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>#465a33</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>#5d7c46</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>#272c21</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>0x479c36</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>10</v>
+      </c>
+      <c r="C34" t="n">
+        <v>46247</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.007388878329931257</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.8575614007435771</v>
+      </c>
+      <c r="F34" t="n">
+        <v>194.4923095703125</v>
+      </c>
+      <c r="G34" t="n">
+        <v>78.82086181640625</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>(0.36470588235294116, 0.48627450980392156, 0.2784313725490196)</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>(0.27450980392156865, 0.3607843137254902, 0.19215686274509805)</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>(0.19607843137254902, 0.23137254901960785, 0.16470588235294117)</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>(0.3176470588235294, 0.42745098039215684, 0.23529411764705882)</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>#5d7c47</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>#465c31</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>#323b2a</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>#516d3c</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>0x49e037</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>day_20.png</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>11</v>
+      </c>
+      <c r="C35" t="n">
+        <v>46725.5</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.007566300958637341</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.9443787580213229</v>
+      </c>
+      <c r="F35" t="n">
+        <v>229.3277435302734</v>
+      </c>
+      <c r="G35" t="n">
+        <v>69.19615173339844</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>(0.36470588235294116, 0.4745098039215686, 0.23921568627450981)</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>(0.5137254901960784, 0.6627450980392157, 0.32941176470588235)</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>(0.21568627450980393, 0.24313725490196078, 0.1843137254901961)</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>(0.44313725490196076, 0.5764705882352941, 0.28627450980392155)</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>#5d793d</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>#83a954</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>#373e2f</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>#719349</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>0x627d02</t>
         </is>
       </c>
     </row>

</xml_diff>